<commit_message>
integracion de los 3 codigos
</commit_message>
<xml_diff>
--- a/generador_de_horarios/MallaCurricular.xlsx
+++ b/generador_de_horarios/MallaCurricular.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvar\Downloads\recomendador-de-horarios-UDP\generador_ruta_critica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Flores\Desktop\grafos\Proyecto semestral\recomendador-de-horarios-UDP\generador_de_horarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9285A9E4-41C0-45A2-8E1F-0B12872E6960}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE1E7EA-240C-4CEC-AA1E-B505AA8A6973}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -273,9 +272,6 @@
     <t>CONTABILIDAD Y COSTOS</t>
   </si>
   <si>
-    <t>INTRODUCCIÓN A LA ECONOMÍA</t>
-  </si>
-  <si>
     <t>OPTIMIZACIÓN</t>
   </si>
   <si>
@@ -355,13 +351,16 @@
   </si>
   <si>
     <t>ELECTRÓNICA Y ELECTROTECNIA</t>
+  </si>
+  <si>
+    <t>INTRODUCCIÓN  A LA ECONOMÍA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -379,6 +378,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -502,7 +509,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -545,9 +552,10 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
+    <cellStyle name="Cálculo" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -575,7 +583,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -873,11 +881,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC6E64A-71CB-4B98-A7E7-F4D52075C1FC}">
   <dimension ref="A2:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
@@ -963,7 +971,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D6" s="12">
         <v>9</v>
@@ -980,7 +988,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D7" s="12">
         <v>38</v>
@@ -1048,7 +1056,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>57</v>
@@ -1133,7 +1141,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D16" s="14">
         <v>19</v>
@@ -1150,7 +1158,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>59</v>
@@ -1167,7 +1175,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>60</v>
@@ -1218,7 +1226,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>61</v>
@@ -1252,7 +1260,7 @@
         <v>18</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D23" s="15">
         <v>27</v>
@@ -1269,7 +1277,7 @@
         <v>19</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D24" s="16">
         <v>29</v>
@@ -1286,7 +1294,7 @@
         <v>20</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D25" s="23" t="s">
         <v>62</v>
@@ -1303,7 +1311,7 @@
         <v>21</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D26" s="16" t="s">
         <v>63</v>
@@ -1320,7 +1328,7 @@
         <v>22</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D27" s="16" t="s">
         <v>64</v>
@@ -1354,7 +1362,7 @@
         <v>23</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D29" s="27">
         <v>0</v>
@@ -1370,8 +1378,8 @@
       <c r="B30" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="6" t="s">
-        <v>79</v>
+      <c r="C30" s="42" t="s">
+        <v>106</v>
       </c>
       <c r="D30" s="28">
         <v>0</v>
@@ -1388,7 +1396,7 @@
         <v>25</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D31" s="28">
         <v>0</v>
@@ -1405,7 +1413,7 @@
         <v>26</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D32" s="17">
         <v>35</v>
@@ -1422,7 +1430,7 @@
         <v>27</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D33" s="17">
         <v>40</v>
@@ -1439,7 +1447,7 @@
         <v>28</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D34" s="17">
         <v>37</v>
@@ -1473,7 +1481,7 @@
         <v>30</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D36" s="18" t="s">
         <v>65</v>
@@ -1490,7 +1498,7 @@
         <v>31</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D37" s="18">
         <v>41</v>
@@ -1507,7 +1515,7 @@
         <v>32</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D38" s="26">
         <v>0</v>
@@ -1524,7 +1532,7 @@
         <v>33</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D39" s="26">
         <v>0</v>
@@ -1541,7 +1549,7 @@
         <v>34</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D40" s="21">
         <v>0</v>
@@ -1558,7 +1566,7 @@
         <v>35</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D41" s="21">
         <v>0</v>
@@ -1575,7 +1583,7 @@
         <v>36</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D42" s="21">
         <v>0</v>
@@ -1592,7 +1600,7 @@
         <v>37</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D43" s="19">
         <v>46</v>
@@ -1677,7 +1685,7 @@
         <v>42</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D48" s="20">
         <v>51</v>
@@ -1762,7 +1770,7 @@
         <v>47</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D53" s="24">
         <v>0</v>

</xml_diff>